<commit_message>
Error in QTN calculation
Middle of fixing error with calculating frequencies of QTNs in
inversions. Currently will calculate frequencies but would include
whether the qtn is found both within and outside of the inversion. Need
those to be separate.
</commit_message>
<xml_diff>
--- a/src/Output_Files_Headers.xlsx
+++ b/src/Output_Files_Headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraschaal/Documents/Northeastern/LotterhosLab/Coding/SLiM/CoreSim_QTL/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C14D466-60BC-1B41-948E-E4C4ABCDF62D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25166057-8734-014B-A4D1-ED3751FA5567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="24480" windowHeight="16160" xr2:uid="{A73851F9-999D-0648-BA32-222C9654DC1C}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="23900" windowHeight="16160" xr2:uid="{A73851F9-999D-0648-BA32-222C9654DC1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>QTN_pos</t>
   </si>
@@ -63,9 +63,6 @@
     <t>qtn_gen_origin</t>
   </si>
   <si>
-    <t>QTN_id</t>
-  </si>
-  <si>
     <t>Summary_Output</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>QTNINV_File</t>
   </si>
   <si>
-    <t>generation</t>
-  </si>
-  <si>
     <t>#_Inv_mutations</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>localAdaptLF_P2</t>
   </si>
   <si>
-    <t>meanQTNFST</t>
-  </si>
-  <si>
     <t>upCIQTNFST</t>
   </si>
   <si>
@@ -225,10 +216,76 @@
     <t>mean_QTNDom</t>
   </si>
   <si>
-    <t>sd_QTNSel</t>
-  </si>
-  <si>
-    <t>sd_QTNDom</t>
+    <t>QTNMutation_Output</t>
+  </si>
+  <si>
+    <t>mut_id</t>
+  </si>
+  <si>
+    <t>mut_pos</t>
+  </si>
+  <si>
+    <t>mut_selCoef</t>
+  </si>
+  <si>
+    <t>mut_originGen</t>
+  </si>
+  <si>
+    <t>freq_p1</t>
+  </si>
+  <si>
+    <t>freq_p2</t>
+  </si>
+  <si>
+    <t>adaptPhenoDiv</t>
+  </si>
+  <si>
+    <t>FST</t>
+  </si>
+  <si>
+    <t>VCF_File</t>
+  </si>
+  <si>
+    <t>heterozygosity</t>
+  </si>
+  <si>
+    <t>homozygosity</t>
+  </si>
+  <si>
+    <t>Inv_Het_Hom</t>
+  </si>
+  <si>
+    <t>Individual_Pheno</t>
+  </si>
+  <si>
+    <t>Individual_id</t>
+  </si>
+  <si>
+    <t>subpop</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>(can merge with INV_MetaData at the end using inv_id)</t>
+  </si>
+  <si>
+    <t>need a question answered to finish</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>not done yet</t>
+  </si>
+  <si>
+    <t>meanQTNINVFST</t>
+  </si>
+  <si>
+    <t>invFST</t>
+  </si>
+  <si>
+    <t>QTN_FST</t>
   </si>
 </sst>
 </file>
@@ -260,12 +317,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -280,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -288,6 +369,29 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -604,150 +708,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FA9F7B-758C-4D40-8F38-7AACC2F9213E}">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" customWidth="1"/>
     <col min="15" max="15" width="13.1640625" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -756,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -767,161 +868,272 @@
       <c r="F12" t="s">
         <v>7</v>
       </c>
+      <c r="G12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="6">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>32</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" t="s">
         <v>33</v>
       </c>
-      <c r="H15" t="s">
+      <c r="K15" t="s">
         <v>34</v>
       </c>
-      <c r="I15" t="s">
+      <c r="L15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" t="s">
         <v>35</v>
       </c>
-      <c r="J15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="P15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>40</v>
+      </c>
+      <c r="R15" t="s">
         <v>41</v>
       </c>
-      <c r="M15" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" t="s">
-        <v>38</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="S15" t="s">
         <v>42</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="T15" t="s">
         <v>43</v>
       </c>
-      <c r="R15" t="s">
+      <c r="U15" t="s">
         <v>44</v>
       </c>
-      <c r="S15" t="s">
+      <c r="V15" t="s">
         <v>45</v>
       </c>
-      <c r="T15" t="s">
+      <c r="W15" t="s">
         <v>46</v>
       </c>
-      <c r="U15" t="s">
+      <c r="X15" t="s">
         <v>47</v>
       </c>
-      <c r="V15" t="s">
+      <c r="Y15" t="s">
         <v>48</v>
-      </c>
-      <c r="W15" t="s">
-        <v>49</v>
-      </c>
-      <c r="X15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="7">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>14</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>16</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>17</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>18</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>19</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>20</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>21</v>
-      </c>
-      <c r="M19" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="7">
         <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="7">
         <v>3</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="13"/>
+      <c r="E38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="8"/>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D40" s="12"/>
+      <c r="E40" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update parameters and edit script to handle no inversions
</commit_message>
<xml_diff>
--- a/src/Output_Files_Headers.xlsx
+++ b/src/Output_Files_Headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraschaal/Documents/Northeastern/LotterhosLab/Coding/SLiM/CoreSim_QTL/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25166057-8734-014B-A4D1-ED3751FA5567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B272DB3-4BED-1B46-9E0E-CE3CB33CC6FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="23900" windowHeight="16160" xr2:uid="{A73851F9-999D-0648-BA32-222C9654DC1C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26160" windowHeight="16160" xr2:uid="{A73851F9-999D-0648-BA32-222C9654DC1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
-  <si>
-    <t>QTN_pos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
   <si>
     <t>inv_pos</t>
   </si>
@@ -42,36 +39,12 @@
     <t>sim_gen</t>
   </si>
   <si>
-    <t>QTN_dom</t>
-  </si>
-  <si>
-    <t>QTN_selCoef</t>
-  </si>
-  <si>
-    <t>QTN_freqP1</t>
-  </si>
-  <si>
-    <t>QTN_freqP2</t>
-  </si>
-  <si>
-    <t>QTN_freq</t>
-  </si>
-  <si>
-    <t>inv_gen_origin</t>
-  </si>
-  <si>
     <t>qtn_gen_origin</t>
   </si>
   <si>
     <t>Summary_Output</t>
   </si>
   <si>
-    <t>mig1</t>
-  </si>
-  <si>
-    <t>mig2</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -99,45 +72,12 @@
     <t>ENVAR</t>
   </si>
   <si>
-    <t>QTNsINV_MetaData_File</t>
-  </si>
-  <si>
-    <t>Population_Dynamics_File</t>
-  </si>
-  <si>
-    <t>QTNINV_File</t>
-  </si>
-  <si>
-    <t>#_Inv_mutations</t>
-  </si>
-  <si>
     <t>Every 200 generations</t>
   </si>
   <si>
     <t>End of Sim</t>
   </si>
   <si>
-    <t>localAdaptSA</t>
-  </si>
-  <si>
-    <t>localAdaptHA_P1</t>
-  </si>
-  <si>
-    <t>localAdaptHA_P2</t>
-  </si>
-  <si>
-    <t>localAdaptLF_P1</t>
-  </si>
-  <si>
-    <t>localAdaptLF_P2</t>
-  </si>
-  <si>
-    <t>upCIQTNFST</t>
-  </si>
-  <si>
-    <t>lowCIQTNFST</t>
-  </si>
-  <si>
     <t>meanNeutFST</t>
   </si>
   <si>
@@ -183,9 +123,6 @@
     <t>SEED</t>
   </si>
   <si>
-    <t>INV_MetaData</t>
-  </si>
-  <si>
     <t>inv_id</t>
   </si>
   <si>
@@ -198,9 +135,6 @@
     <t>inv_originGen</t>
   </si>
   <si>
-    <t>INV_File</t>
-  </si>
-  <si>
     <t>freq</t>
   </si>
   <si>
@@ -210,12 +144,6 @@
     <t>freq_P2</t>
   </si>
   <si>
-    <t>mean_QTNSelCoef</t>
-  </si>
-  <si>
-    <t>mean_QTNDom</t>
-  </si>
-  <si>
     <t>QTNMutation_Output</t>
   </si>
   <si>
@@ -249,9 +177,6 @@
     <t>heterozygosity</t>
   </si>
   <si>
-    <t>homozygosity</t>
-  </si>
-  <si>
     <t>Inv_Het_Hom</t>
   </si>
   <si>
@@ -279,13 +204,97 @@
     <t>not done yet</t>
   </si>
   <si>
-    <t>meanQTNINVFST</t>
-  </si>
-  <si>
     <t>invFST</t>
   </si>
   <si>
-    <t>QTN_FST</t>
+    <t>MIG1</t>
+  </si>
+  <si>
+    <t>MIG2</t>
+  </si>
+  <si>
+    <t>?input</t>
+  </si>
+  <si>
+    <t>locAdaptSA</t>
+  </si>
+  <si>
+    <t>locAdaptHAP1</t>
+  </si>
+  <si>
+    <t>locAdaptHAP2</t>
+  </si>
+  <si>
+    <t>locAdaptLFP1</t>
+  </si>
+  <si>
+    <t>locAdaptLFP2</t>
+  </si>
+  <si>
+    <t>Num_Inv_mutations</t>
+  </si>
+  <si>
+    <t>qtn_pos</t>
+  </si>
+  <si>
+    <t>qtn_selCoef</t>
+  </si>
+  <si>
+    <t>qtn_dom</t>
+  </si>
+  <si>
+    <t>num_qtns</t>
+  </si>
+  <si>
+    <t>mean_qtnSelCoef</t>
+  </si>
+  <si>
+    <t>sd_qtnSelCoef</t>
+  </si>
+  <si>
+    <t>mean_qtnDom</t>
+  </si>
+  <si>
+    <t>sd_qtnDom</t>
+  </si>
+  <si>
+    <t>_outputInvSumInfo.txt</t>
+  </si>
+  <si>
+    <t>_outputInvTime.txt</t>
+  </si>
+  <si>
+    <t>_outputInvQtnSumInfo.txt</t>
+  </si>
+  <si>
+    <t>_outputPopDynam.txt</t>
+  </si>
+  <si>
+    <t>qtn_id</t>
+  </si>
+  <si>
+    <t>_outputInvQtn.txt</t>
+  </si>
+  <si>
+    <t>qtn_freqP1</t>
+  </si>
+  <si>
+    <t>qtn_freqP2</t>
+  </si>
+  <si>
+    <t>qtn_freq</t>
+  </si>
+  <si>
+    <t>qtn_FST</t>
+  </si>
+  <si>
+    <t>meanQtnInvWinFST</t>
+  </si>
+  <si>
+    <t>upCIQtnInvFST</t>
+  </si>
+  <si>
+    <t>lowCIQtnInvFST</t>
   </si>
 </sst>
 </file>
@@ -344,7 +353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,39 +370,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FA9F7B-758C-4D40-8F38-7AACC2F9213E}">
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:AV40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,11 +715,12 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" customWidth="1"/>
     <col min="15" max="15" width="13.1640625" customWidth="1"/>
@@ -734,335 +730,373 @@
     <col min="23" max="23" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:48" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="W15" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="X15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="11"/>
+      <c r="AR15" s="11"/>
+      <c r="AS15" s="11"/>
+      <c r="AT15" s="11"/>
+      <c r="AU15" s="11"/>
+      <c r="AV15" s="11"/>
+    </row>
+    <row r="17" spans="1:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" t="s">
-        <v>37</v>
-      </c>
-      <c r="N15" t="s">
-        <v>36</v>
-      </c>
-      <c r="O15" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>40</v>
-      </c>
-      <c r="R15" t="s">
-        <v>41</v>
-      </c>
-      <c r="S15" t="s">
-        <v>42</v>
-      </c>
-      <c r="T15" t="s">
-        <v>43</v>
-      </c>
-      <c r="U15" t="s">
-        <v>44</v>
-      </c>
-      <c r="V15" t="s">
-        <v>45</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="X15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1074,66 +1108,67 @@
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
+      <c r="A27" s="4">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="10" t="s">
-        <v>75</v>
+      <c r="A28" s="1"/>
+      <c r="B28" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="11">
+      <c r="A30" s="4">
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D38" s="13"/>
+      <c r="D38" s="8"/>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D39" s="8"/>
+      <c r="D39" s="5"/>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D40" s="12"/>
+      <c r="D40" s="7"/>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New figures and sim scripts
</commit_message>
<xml_diff>
--- a/src/Output_Files_Headers.xlsx
+++ b/src/Output_Files_Headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraschaal/Documents/Northeastern/LotterhosLab/Coding/SLiM/CoreSim_QTL/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4181238A-39C1-444E-8C93-B391D7816DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB8BF7A-9FAB-C749-9460-B20437D017F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26160" windowHeight="16160" xr2:uid="{A73851F9-999D-0648-BA32-222C9654DC1C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>inv_pos</t>
   </si>
@@ -171,12 +171,6 @@
     <t>FST</t>
   </si>
   <si>
-    <t>heterozygosity</t>
-  </si>
-  <si>
-    <t>Inv_Het_Hom</t>
-  </si>
-  <si>
     <t>Individual_Pheno</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>phenotype</t>
   </si>
   <si>
-    <t>(can merge with INV_MetaData at the end using inv_id)</t>
-  </si>
-  <si>
     <t>need a question answered to finish</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>MIG2</t>
   </si>
   <si>
-    <t>?input</t>
-  </si>
-  <si>
     <t>locAdaptSA</t>
   </si>
   <si>
@@ -285,16 +273,25 @@
     <t>qtn_FST</t>
   </si>
   <si>
-    <t>meanQtnInvWinFST</t>
-  </si>
-  <si>
-    <t>upCIQtnInvFST</t>
-  </si>
-  <si>
-    <t>lowCIQtnInvFST</t>
-  </si>
-  <si>
     <t>_InversionQTL.vcf</t>
+  </si>
+  <si>
+    <t>meanQtnFST</t>
+  </si>
+  <si>
+    <t>upCIQtnFST</t>
+  </si>
+  <si>
+    <t>lowCIQtnFST</t>
+  </si>
+  <si>
+    <t>all QTNs</t>
+  </si>
+  <si>
+    <t>all Inversions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all neutral </t>
   </si>
 </sst>
 </file>
@@ -381,7 +378,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -389,6 +385,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FA9F7B-758C-4D40-8F38-7AACC2F9213E}">
   <dimension ref="A1:AV40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,27 +737,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -772,42 +769,42 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>56</v>
+      <c r="L6" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.2">
@@ -818,31 +815,31 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>68</v>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.2">
@@ -853,31 +850,31 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>83</v>
+      <c r="H12" s="10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.2">
@@ -888,105 +885,114 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="L15" s="11" t="s">
+      <c r="I15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="N15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="O15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="P15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="11" t="s">
+      <c r="Q15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="R15" s="11" t="s">
+      <c r="R15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="S15" s="11" t="s">
+      <c r="S15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="11" t="s">
+      <c r="T15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="U15" s="11" t="s">
+      <c r="U15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="V15" s="11" t="s">
+      <c r="V15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W15" s="11" t="s">
+      <c r="W15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="X15" s="11" t="s">
+      <c r="X15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Y15" s="11" t="s">
+      <c r="Y15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AN15" s="11"/>
-      <c r="AO15" s="11"/>
-      <c r="AP15" s="11"/>
-      <c r="AQ15" s="11"/>
-      <c r="AR15" s="11"/>
-      <c r="AS15" s="11"/>
-      <c r="AT15" s="11"/>
-      <c r="AU15" s="11"/>
-      <c r="AV15" s="11"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="10"/>
+      <c r="AJ15" s="10"/>
+      <c r="AK15" s="10"/>
+      <c r="AL15" s="10"/>
+      <c r="AM15" s="10"/>
+      <c r="AN15" s="10"/>
+      <c r="AO15" s="10"/>
+      <c r="AP15" s="10"/>
+      <c r="AQ15" s="10"/>
+      <c r="AR15" s="10"/>
+      <c r="AS15" s="10"/>
+      <c r="AT15" s="10"/>
+      <c r="AU15" s="10"/>
+      <c r="AV15" s="10"/>
     </row>
     <row r="17" spans="1:13" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -1000,46 +1006,43 @@
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" t="s">
+      <c r="B19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1056,37 +1059,35 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" s="10"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
@@ -1096,15 +1097,15 @@
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -1112,63 +1113,48 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>46</v>
-      </c>
+      <c r="A30" s="8"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D38" s="8"/>
+      <c r="D38" s="7"/>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D39" s="5"/>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D40" s="7"/>
+      <c r="D40" s="6"/>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>